<commit_message>
Add missing Documents validation test case to tracker
</commit_message>
<xml_diff>
--- a/TEST_TRACKER_TEMPLATE.xlsx
+++ b/TEST_TRACKER_TEMPLATE.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1030,22 +1030,22 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>Member can view/download shared documents</t>
+          <t>Admin document upload validation checks</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>Member</t>
+          <t>Admin</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Open dashboard Documents tab and download a file</t>
+          <t>Try unsupported extension or oversize file on admin upload form</t>
         </is>
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>Document list is visible and download works</t>
+          <t>Specific validation error appears and file is not added</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
@@ -1062,17 +1062,17 @@
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>ARC-01</t>
+          <t>DOC-03</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>Archive</t>
+          <t>Documents</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>Member uploads own archive file</t>
+          <t>Member can view/download shared documents</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
@@ -1082,12 +1082,12 @@
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>In Archive tab upload a valid file with optional folder name</t>
+          <t>Open dashboard Documents tab and download a file</t>
         </is>
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>Upload succeeds and file appears in personal list</t>
+          <t>Document list is visible and download works</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
@@ -1104,7 +1104,7 @@
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>ARC-02</t>
+          <t>ARC-01</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1114,22 +1114,22 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>Archive privacy between members</t>
+          <t>Member uploads own archive file</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>Member A and Member B</t>
+          <t>Member</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Upload as Member A, then login as Member B and check archive list/download</t>
+          <t>In Archive tab upload a valid file with optional folder name</t>
         </is>
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>Member B cannot see or access Member A files</t>
+          <t>Upload succeeds and file appears in personal list</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
@@ -1146,7 +1146,7 @@
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>ARC-03</t>
+          <t>ARC-02</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1156,22 +1156,22 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>Archive validation handling</t>
+          <t>Archive privacy between members</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>Member</t>
+          <t>Member A and Member B</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>Try unsupported extension or oversize file</t>
+          <t>Upload as Member A, then login as Member B and check archive list/download</t>
         </is>
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>Specific error notice shown (type/size/quota) and no file added</t>
+          <t>Member B cannot see or access Member A files</t>
         </is>
       </c>
       <c r="G17" s="2" t="inlineStr">
@@ -1188,17 +1188,17 @@
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>FND-01</t>
+          <t>ARC-03</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>Funding</t>
+          <t>Archive</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>Member submits funding request</t>
+          <t>Archive validation handling</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
@@ -1208,12 +1208,12 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Create a funding request from dashboard</t>
+          <t>Try unsupported extension or oversize file</t>
         </is>
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>Request saves and confirmation appears</t>
+          <t>Specific error notice shown (type/size/quota) and no file added</t>
         </is>
       </c>
       <c r="G18" s="2" t="inlineStr">
@@ -1230,7 +1230,7 @@
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>FND-02</t>
+          <t>FND-01</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1240,22 +1240,22 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>Admin reviews funding request</t>
+          <t>Member submits funding request</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>Member</t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>Open LoveKin Funding Requests and review submitted request</t>
+          <t>Create a funding request from dashboard</t>
         </is>
       </c>
       <c r="F19" s="2" t="inlineStr">
         <is>
-          <t>Admin can view request details and status</t>
+          <t>Request saves and confirmation appears</t>
         </is>
       </c>
       <c r="G19" s="2" t="inlineStr">
@@ -1272,32 +1272,32 @@
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>REP-01</t>
+          <t>FND-02</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>Reports</t>
+          <t>Funding</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>Reports visibility by role</t>
+          <t>Admin reviews funding request</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>Admin and Member</t>
+          <t>Admin</t>
         </is>
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Open Reports tab for different roles</t>
+          <t>Open LoveKin Funding Requests and review submitted request</t>
         </is>
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>Each role sees expected report access/data</t>
+          <t>Admin can view request details and status</t>
         </is>
       </c>
       <c r="G20" s="2" t="inlineStr">
@@ -1314,32 +1314,32 @@
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>TLS-01</t>
+          <t>REP-01</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>Tools</t>
+          <t>Reports</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>Generate demo data</t>
+          <t>Reports visibility by role</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>Admin</t>
+          <t>Admin and Member</t>
         </is>
       </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>Go to LoveKin Tools and click Generate Demo Data</t>
+          <t>Open Reports tab for different roles</t>
         </is>
       </c>
       <c r="F21" s="2" t="inlineStr">
         <is>
-          <t>6 demo records are created per core dataset</t>
+          <t>Each role sees expected report access/data</t>
         </is>
       </c>
       <c r="G21" s="2" t="inlineStr">
@@ -1356,7 +1356,7 @@
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>TLS-02</t>
+          <t>TLS-01</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>Generate demo data rerun reset</t>
+          <t>Generate demo data</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
@@ -1376,12 +1376,12 @@
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Click Generate Demo Data again</t>
+          <t>Go to LoveKin Tools and click Generate Demo Data</t>
         </is>
       </c>
       <c r="F22" s="2" t="inlineStr">
         <is>
-          <t>Old demo records are reset and recreated (no duplicates)</t>
+          <t>6 demo records are created per core dataset</t>
         </is>
       </c>
       <c r="G22" s="2" t="inlineStr">
@@ -1398,7 +1398,7 @@
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>TLS-03</t>
+          <t>TLS-02</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>Erase demo content</t>
+          <t>Generate demo data rerun reset</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
@@ -1418,12 +1418,12 @@
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>Click Erase Demo Content and confirm</t>
+          <t>Click Generate Demo Data again</t>
         </is>
       </c>
       <c r="F23" s="2" t="inlineStr">
         <is>
-          <t>Only demo-tagged records are deleted</t>
+          <t>Old demo records are reset and recreated (no duplicates)</t>
         </is>
       </c>
       <c r="G23" s="2" t="inlineStr">
@@ -1440,32 +1440,32 @@
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>UI-01</t>
+          <t>TLS-03</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>UI</t>
+          <t>Tools</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>Desktop and mobile visual check</t>
+          <t>Erase demo content</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>Member</t>
+          <t>Admin</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>Review login/register/dashboard documents and archive on desktop and phone widths</t>
+          <t>Click Erase Demo Content and confirm</t>
         </is>
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>Layout is readable, aligned, and functional</t>
+          <t>Only demo-tagged records are deleted</t>
         </is>
       </c>
       <c r="G24" s="2" t="inlineStr">
@@ -1479,6 +1479,48 @@
       <c r="K24" s="2" t="inlineStr"/>
       <c r="L24" s="2" t="inlineStr"/>
     </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>UI-01</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>UI</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>Desktop and mobile visual check</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>Member</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>Review login/register/dashboard documents and archive on desktop and phone widths</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>Layout is readable, aligned, and functional</t>
+        </is>
+      </c>
+      <c r="G25" s="2" t="inlineStr">
+        <is>
+          <t>NOT RUN</t>
+        </is>
+      </c>
+      <c r="H25" s="2" t="inlineStr"/>
+      <c r="I25" s="2" t="inlineStr"/>
+      <c r="J25" s="2" t="inlineStr"/>
+      <c r="K25" s="2" t="inlineStr"/>
+      <c r="L25" s="2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>